<commit_message>
added 1s and 2s of Cl in ice
</commit_message>
<xml_diff>
--- a/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_ccsd.xlsx
+++ b/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_ccsd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/github_thesis_graph/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C7E87D-6B2C-DC40-A23B-A3A2BB3466D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C48D963-211C-3B45-AEFC-DFAE4F5EFEBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1240" windowWidth="21640" windowHeight="14420" xr2:uid="{41A0B090-B6CC-EE4B-87B1-C158C411CEA8}"/>
+    <workbookView xWindow="3960" yWindow="960" windowWidth="21640" windowHeight="14420" xr2:uid="{41A0B090-B6CC-EE4B-87B1-C158C411CEA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,453 +388,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894879FA-00C2-5D46-B04A-A85BFC6EEBFA}">
-  <dimension ref="B3:R28"/>
+  <dimension ref="B4:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>2833.047536</v>
-      </c>
-      <c r="F4">
-        <v>275.4979932</v>
-      </c>
-      <c r="J4">
-        <v>204.09148329999999</v>
-      </c>
-      <c r="N4">
-        <v>204.93894230000001</v>
-      </c>
-      <c r="R4">
-        <v>203.24402430000001</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>2832.5795400000002</v>
+        <v>2833.047536</v>
       </c>
       <c r="F5">
-        <v>275.06690889999999</v>
+        <v>275.4979932</v>
       </c>
       <c r="J5">
-        <v>203.65773669999999</v>
+        <v>204.09148329999999</v>
       </c>
       <c r="N5">
-        <v>204.50507210000001</v>
+        <v>204.93894230000001</v>
       </c>
       <c r="R5">
-        <v>202.8104013</v>
+        <v>203.24402430000001</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>2832.9288999999999</v>
+        <v>2832.5795400000002</v>
       </c>
       <c r="F6">
-        <v>275.4191343</v>
+        <v>275.06690889999999</v>
       </c>
       <c r="J6">
-        <v>204.00988469999999</v>
+        <v>203.65773669999999</v>
       </c>
       <c r="N6">
-        <v>204.85720889999999</v>
+        <v>204.50507210000001</v>
       </c>
       <c r="R6">
-        <v>203.16256039999999</v>
+        <v>202.8104013</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>2828.3437869999998</v>
+        <v>2832.9288999999999</v>
       </c>
       <c r="F7">
-        <v>270.92929129999999</v>
+        <v>275.4191343</v>
       </c>
       <c r="J7">
-        <v>199.5458936</v>
+        <v>204.00988469999999</v>
       </c>
       <c r="N7">
-        <v>200.3933681</v>
+        <v>204.85720889999999</v>
       </c>
       <c r="R7">
-        <v>198.69841919999999</v>
+        <v>203.16256039999999</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>2832.9579530000001</v>
+        <v>2828.3437869999998</v>
       </c>
       <c r="F8">
-        <v>275.43790230000002</v>
+        <v>270.92929129999999</v>
       </c>
       <c r="J8">
-        <v>204.02943089999999</v>
+        <v>199.5458936</v>
       </c>
       <c r="N8">
-        <v>204.8767986</v>
+        <v>200.3933681</v>
       </c>
       <c r="R8">
-        <v>203.18206319999999</v>
+        <v>198.69841919999999</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>2831.4584789999999</v>
+        <v>2832.9579530000001</v>
       </c>
       <c r="F9">
-        <v>273.89570529999997</v>
+        <v>275.43790230000002</v>
       </c>
       <c r="J9">
-        <v>202.4906579</v>
+        <v>204.02943089999999</v>
       </c>
       <c r="N9">
-        <v>203.33816809999999</v>
+        <v>204.8767986</v>
       </c>
       <c r="R9">
-        <v>201.64314759999999</v>
+        <v>203.18206319999999</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>2832.3558539999999</v>
+        <v>2831.4584789999999</v>
       </c>
       <c r="F10">
-        <v>274.83998550000001</v>
+        <v>273.89570529999997</v>
       </c>
       <c r="J10">
-        <v>203.43131600000001</v>
+        <v>202.4906579</v>
       </c>
       <c r="N10">
-        <v>204.27865650000001</v>
+        <v>203.33816809999999</v>
       </c>
       <c r="R10">
-        <v>202.58397550000001</v>
+        <v>201.64314759999999</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>2832.4917639999999</v>
+        <v>2832.3558539999999</v>
       </c>
       <c r="F11">
-        <v>274.94197229999997</v>
+        <v>274.83998550000001</v>
       </c>
       <c r="J11">
-        <v>203.53579110000001</v>
+        <v>203.43131600000001</v>
       </c>
       <c r="N11">
-        <v>204.38323539999999</v>
+        <v>204.27865650000001</v>
       </c>
       <c r="R11">
-        <v>202.6883469</v>
+        <v>202.58397550000001</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>2832.6044019999999</v>
+        <v>2832.4917639999999</v>
       </c>
       <c r="F12">
-        <v>275.07372420000002</v>
+        <v>274.94197229999997</v>
       </c>
       <c r="J12">
-        <v>203.6657251</v>
+        <v>203.53579110000001</v>
       </c>
       <c r="N12">
-        <v>204.51311000000001</v>
+        <v>204.38323539999999</v>
       </c>
       <c r="R12">
-        <v>202.81834019999999</v>
+        <v>202.6883469</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>2831.7597190000001</v>
+        <v>2832.6044019999999</v>
       </c>
       <c r="F13">
-        <v>274.21060949999998</v>
+        <v>275.07372420000002</v>
       </c>
       <c r="J13">
-        <v>202.80417990000001</v>
+        <v>203.6657251</v>
       </c>
       <c r="N13">
-        <v>203.65162710000001</v>
+        <v>204.51311000000001</v>
       </c>
       <c r="R13">
-        <v>201.95673260000001</v>
+        <v>202.81834019999999</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>2831.646671</v>
+        <v>2831.7597190000001</v>
       </c>
       <c r="F14">
-        <v>274.08242089999999</v>
+        <v>274.21060949999998</v>
       </c>
       <c r="J14">
-        <v>202.6769942</v>
+        <v>202.80417990000001</v>
       </c>
       <c r="N14">
-        <v>203.52450390000001</v>
+        <v>203.65162710000001</v>
       </c>
       <c r="R14">
-        <v>201.8294846</v>
+        <v>201.95673260000001</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>2831.613331</v>
+        <v>2831.646671</v>
       </c>
       <c r="F15">
-        <v>274.05881049999999</v>
+        <v>274.08242089999999</v>
       </c>
       <c r="J15">
-        <v>202.6525096</v>
+        <v>202.6769942</v>
       </c>
       <c r="N15">
-        <v>203.4999895</v>
+        <v>203.52450390000001</v>
       </c>
       <c r="R15">
-        <v>201.80502960000001</v>
+        <v>201.8294846</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>2831.9260439999998</v>
+        <v>2831.613331</v>
       </c>
       <c r="F16">
-        <v>274.41097710000003</v>
+        <v>274.05881049999999</v>
       </c>
       <c r="J16">
-        <v>203.0020251</v>
+        <v>202.6525096</v>
       </c>
       <c r="N16">
-        <v>203.84937360000001</v>
+        <v>203.4999895</v>
       </c>
       <c r="R16">
-        <v>202.15467659999999</v>
+        <v>201.80502960000001</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>2832.713816</v>
+        <v>2831.9260439999998</v>
       </c>
       <c r="F17">
-        <v>275.17934939999998</v>
+        <v>274.41097710000003</v>
       </c>
       <c r="J17">
-        <v>203.77192450000001</v>
+        <v>203.0020251</v>
       </c>
       <c r="N17">
-        <v>204.6193241</v>
+        <v>203.84937360000001</v>
       </c>
       <c r="R17">
-        <v>202.92452499999999</v>
+        <v>202.15467659999999</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>2832.9569449999999</v>
+        <v>2832.713816</v>
       </c>
       <c r="F18">
-        <v>275.44506339999998</v>
+        <v>275.17934939999998</v>
       </c>
       <c r="J18">
-        <v>204.0359254</v>
+        <v>203.77192450000001</v>
       </c>
       <c r="N18">
-        <v>204.88325309999999</v>
+        <v>204.6193241</v>
       </c>
       <c r="R18">
-        <v>203.1885977</v>
+        <v>202.92452499999999</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>2832.2236290000001</v>
+        <v>2832.9569449999999</v>
       </c>
       <c r="F19">
-        <v>274.67940959999999</v>
+        <v>275.44506339999998</v>
       </c>
       <c r="J19">
-        <v>203.27288490000001</v>
+        <v>204.0359254</v>
       </c>
       <c r="N19">
-        <v>204.1203094</v>
+        <v>204.88325309999999</v>
       </c>
       <c r="R19">
-        <v>202.42546039999999</v>
+        <v>203.1885977</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>2831.8736039999999</v>
+        <v>2832.2236290000001</v>
       </c>
       <c r="F20">
-        <v>274.32325809999998</v>
+        <v>274.67940959999999</v>
       </c>
       <c r="J20">
-        <v>202.91658519999999</v>
+        <v>203.27288490000001</v>
       </c>
       <c r="N20">
-        <v>203.76406489999999</v>
+        <v>204.1203094</v>
       </c>
       <c r="R20">
-        <v>202.06910550000001</v>
+        <v>202.42546039999999</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>2830.8073869999998</v>
+        <v>2831.8736039999999</v>
       </c>
       <c r="F21">
-        <v>273.17381699999999</v>
+        <v>274.32325809999998</v>
       </c>
       <c r="J21">
-        <v>201.81222310000001</v>
+        <v>202.91658519999999</v>
       </c>
       <c r="N21">
-        <v>202.65986179999999</v>
+        <v>203.76406489999999</v>
       </c>
       <c r="R21">
-        <v>200.96458430000001</v>
+        <v>202.06910550000001</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>2832.952127</v>
+        <v>2830.8073869999998</v>
       </c>
       <c r="F22">
-        <v>275.43354260000001</v>
+        <v>273.17381699999999</v>
       </c>
       <c r="J22">
-        <v>204.0247358</v>
+        <v>201.81222310000001</v>
       </c>
       <c r="N22">
-        <v>204.87208759999999</v>
+        <v>202.65986179999999</v>
       </c>
       <c r="R22">
-        <v>203.17738399999999</v>
+        <v>200.96458430000001</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>2833.3361930000001</v>
+        <v>2832.952127</v>
       </c>
       <c r="F23">
-        <v>275.83515569999997</v>
+        <v>275.43354260000001</v>
       </c>
       <c r="J23">
-        <v>204.4249489</v>
+        <v>204.0247358</v>
       </c>
       <c r="N23">
-        <v>205.2722474</v>
+        <v>204.87208759999999</v>
       </c>
       <c r="R23">
-        <v>203.5776505</v>
+        <v>203.17738399999999</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>2831.598105</v>
+        <v>2833.3361930000001</v>
       </c>
       <c r="F24">
-        <v>274.03102639999997</v>
+        <v>275.83515569999997</v>
       </c>
       <c r="J24">
-        <v>202.62565799999999</v>
+        <v>204.4249489</v>
       </c>
       <c r="N24">
-        <v>203.47321120000001</v>
+        <v>205.2722474</v>
       </c>
       <c r="R24">
-        <v>201.77810489999999</v>
+        <v>203.5776505</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>2830.8131079999998</v>
+        <v>2831.598105</v>
       </c>
       <c r="F25">
-        <v>273.19750859999999</v>
+        <v>274.03102639999997</v>
       </c>
       <c r="J25">
-        <v>201.8342351</v>
+        <v>202.62565799999999</v>
       </c>
       <c r="N25">
-        <v>202.68179230000001</v>
+        <v>203.47321120000001</v>
       </c>
       <c r="R25">
-        <v>200.98667789999999</v>
+        <v>201.77810489999999</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>2832.7135969999999</v>
+        <v>2830.8131079999998</v>
       </c>
       <c r="F26">
-        <v>275.20596610000001</v>
+        <v>273.19750859999999</v>
       </c>
       <c r="J26">
-        <v>203.79644859999999</v>
+        <v>201.8342351</v>
       </c>
       <c r="N26">
-        <v>204.6437731</v>
+        <v>202.68179230000001</v>
       </c>
       <c r="R26">
-        <v>202.94912400000001</v>
+        <v>200.98667789999999</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>2832.3486240000002</v>
+        <v>2832.7135969999999</v>
       </c>
       <c r="F27">
-        <v>274.8558041</v>
+        <v>275.20596610000001</v>
       </c>
       <c r="J27">
-        <v>203.4451875</v>
+        <v>203.79644859999999</v>
       </c>
       <c r="N27">
-        <v>204.29248269999999</v>
+        <v>204.6437731</v>
       </c>
       <c r="R27">
-        <v>202.59789230000001</v>
+        <v>202.94912400000001</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28">
+        <v>2832.3486240000002</v>
+      </c>
+      <c r="F28">
+        <v>274.8558041</v>
+      </c>
+      <c r="J28">
+        <v>203.4451875</v>
+      </c>
+      <c r="N28">
+        <v>204.29248269999999</v>
+      </c>
+      <c r="R28">
+        <v>202.59789230000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B29">
         <v>2832.6976800000002</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>275.17209380000003</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>203.76399180000001</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>204.61135609999999</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>202.9166276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Cl- in ice
</commit_message>
<xml_diff>
--- a/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_ccsd.xlsx
+++ b/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_ccsd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C48D963-211C-3B45-AEFC-DFAE4F5EFEBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F53C06-A3B0-284B-B7E8-5FC3DF11615E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="960" windowWidth="21640" windowHeight="14420" xr2:uid="{41A0B090-B6CC-EE4B-87B1-C158C411CEA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Embedded_one_water_1s_cl_acv3z_x2camf</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Embedded_one_water_p12_cl_acv3z_x2camf</t>
+  </si>
+  <si>
+    <t>Embedded_one_water_p32_cl_acv3z_x2camf</t>
   </si>
 </sst>
 </file>
@@ -390,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894879FA-00C2-5D46-B04A-A85BFC6EEBFA}">
   <dimension ref="B4:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">

</xml_diff>